<commit_message>
Exports Import Excel Promotion
</commit_message>
<xml_diff>
--- a/public/Excel/MASTER_DATA.xlsx
+++ b/public/Excel/MASTER_DATA.xlsx
@@ -1039,8 +1039,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AT51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AC2" workbookViewId="0">
-      <selection activeCell="AL2" sqref="AL2:AL24"/>
+    <sheetView tabSelected="1" topLeftCell="AD2" workbookViewId="0">
+      <selection activeCell="AM3" sqref="AM3:AM24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1312,7 +1312,7 @@
         <v>42409</v>
       </c>
       <c r="AM2" s="2">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AN2" s="2" t="s">
         <v>21</v>
@@ -1321,13 +1321,13 @@
         <v>5</v>
       </c>
       <c r="AP2" s="2">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="AQ2" s="2">
-        <v>3000</v>
+        <v>0</v>
       </c>
       <c r="AR2" s="2">
-        <v>4000</v>
+        <v>0</v>
       </c>
       <c r="AS2" s="12">
         <v>1</v>
@@ -1449,7 +1449,7 @@
         <v>42409</v>
       </c>
       <c r="AM3" s="2">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AN3" s="2" t="s">
         <v>38</v>
@@ -1458,13 +1458,13 @@
         <v>5</v>
       </c>
       <c r="AP3" s="2">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="AQ3" s="2">
-        <v>3000</v>
+        <v>0</v>
       </c>
       <c r="AR3" s="2">
-        <v>4000</v>
+        <v>0</v>
       </c>
       <c r="AS3" s="12">
         <v>1</v>
@@ -1586,7 +1586,7 @@
         <v>42409</v>
       </c>
       <c r="AM4" s="2">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AN4" s="2" t="s">
         <v>38</v>
@@ -1595,13 +1595,13 @@
         <v>5</v>
       </c>
       <c r="AP4" s="2">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="AQ4" s="2">
-        <v>3000</v>
+        <v>0</v>
       </c>
       <c r="AR4" s="2">
-        <v>4000</v>
+        <v>0</v>
       </c>
       <c r="AS4" s="12">
         <v>1</v>
@@ -1723,7 +1723,7 @@
         <v>42409</v>
       </c>
       <c r="AM5" s="2">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AN5" s="2" t="s">
         <v>21</v>
@@ -1732,13 +1732,13 @@
         <v>5</v>
       </c>
       <c r="AP5" s="2">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="AQ5" s="2">
-        <v>3000</v>
+        <v>0</v>
       </c>
       <c r="AR5" s="2">
-        <v>4000</v>
+        <v>0</v>
       </c>
       <c r="AS5" s="12">
         <v>1</v>
@@ -1860,7 +1860,7 @@
         <v>42409</v>
       </c>
       <c r="AM6" s="2">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AN6" s="2" t="s">
         <v>71</v>
@@ -1869,13 +1869,13 @@
         <v>5</v>
       </c>
       <c r="AP6" s="2">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="AQ6" s="2">
-        <v>3000</v>
+        <v>0</v>
       </c>
       <c r="AR6" s="2">
-        <v>4000</v>
+        <v>0</v>
       </c>
       <c r="AS6" s="12">
         <v>1</v>
@@ -1997,7 +1997,7 @@
         <v>42409</v>
       </c>
       <c r="AM7" s="2">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AN7" s="2" t="s">
         <v>87</v>
@@ -2006,13 +2006,13 @@
         <v>5</v>
       </c>
       <c r="AP7" s="2">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="AQ7" s="2">
-        <v>3000</v>
+        <v>0</v>
       </c>
       <c r="AR7" s="2">
-        <v>4000</v>
+        <v>0</v>
       </c>
       <c r="AS7" s="12">
         <v>1</v>
@@ -2134,7 +2134,7 @@
         <v>42409</v>
       </c>
       <c r="AM8" s="2">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AN8" s="2" t="s">
         <v>87</v>
@@ -2143,13 +2143,13 @@
         <v>5</v>
       </c>
       <c r="AP8" s="2">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="AQ8" s="2">
-        <v>3000</v>
+        <v>0</v>
       </c>
       <c r="AR8" s="2">
-        <v>4000</v>
+        <v>0</v>
       </c>
       <c r="AS8" s="12">
         <v>1</v>
@@ -2271,7 +2271,7 @@
         <v>42409</v>
       </c>
       <c r="AM9" s="2">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AN9" s="2" t="s">
         <v>87</v>
@@ -2280,13 +2280,13 @@
         <v>5</v>
       </c>
       <c r="AP9" s="2">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="AQ9" s="2">
-        <v>3000</v>
+        <v>0</v>
       </c>
       <c r="AR9" s="2">
-        <v>4000</v>
+        <v>0</v>
       </c>
       <c r="AS9" s="12">
         <v>1</v>
@@ -2408,7 +2408,7 @@
         <v>42409</v>
       </c>
       <c r="AM10" s="2">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AN10" s="2" t="s">
         <v>21</v>
@@ -2417,13 +2417,13 @@
         <v>5</v>
       </c>
       <c r="AP10" s="2">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="AQ10" s="2">
-        <v>3000</v>
+        <v>0</v>
       </c>
       <c r="AR10" s="2">
-        <v>4000</v>
+        <v>0</v>
       </c>
       <c r="AS10" s="12">
         <v>1</v>
@@ -2545,7 +2545,7 @@
         <v>42409</v>
       </c>
       <c r="AM11" s="2">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AN11" s="10" t="s">
         <v>131</v>
@@ -2554,13 +2554,13 @@
         <v>132</v>
       </c>
       <c r="AP11" s="2">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="AQ11" s="2">
-        <v>3000</v>
+        <v>0</v>
       </c>
       <c r="AR11" s="2">
-        <v>4000</v>
+        <v>0</v>
       </c>
       <c r="AS11" s="12">
         <v>1</v>
@@ -2683,7 +2683,7 @@
         <v>42409</v>
       </c>
       <c r="AM12" s="2">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AN12" s="2" t="s">
         <v>21</v>
@@ -2692,13 +2692,13 @@
         <v>5</v>
       </c>
       <c r="AP12" s="2">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="AQ12" s="2">
-        <v>3000</v>
+        <v>0</v>
       </c>
       <c r="AR12" s="2">
-        <v>4000</v>
+        <v>0</v>
       </c>
       <c r="AS12" s="12">
         <v>1</v>
@@ -2821,7 +2821,7 @@
         <v>42409</v>
       </c>
       <c r="AM13" s="2">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AN13" s="2" t="s">
         <v>38</v>
@@ -2830,13 +2830,13 @@
         <v>5</v>
       </c>
       <c r="AP13" s="2">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="AQ13" s="2">
-        <v>3000</v>
+        <v>0</v>
       </c>
       <c r="AR13" s="2">
-        <v>4000</v>
+        <v>0</v>
       </c>
       <c r="AS13" s="12">
         <v>1</v>
@@ -2959,7 +2959,7 @@
         <v>42409</v>
       </c>
       <c r="AM14" s="2">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AN14" s="2" t="s">
         <v>38</v>
@@ -2968,13 +2968,13 @@
         <v>5</v>
       </c>
       <c r="AP14" s="2">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="AQ14" s="2">
-        <v>3000</v>
+        <v>0</v>
       </c>
       <c r="AR14" s="2">
-        <v>4000</v>
+        <v>0</v>
       </c>
       <c r="AS14" s="12">
         <v>1</v>
@@ -3097,7 +3097,7 @@
         <v>42409</v>
       </c>
       <c r="AM15" s="2">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AN15" s="2" t="s">
         <v>21</v>
@@ -3106,13 +3106,13 @@
         <v>5</v>
       </c>
       <c r="AP15" s="2">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="AQ15" s="2">
-        <v>3000</v>
+        <v>0</v>
       </c>
       <c r="AR15" s="2">
-        <v>4000</v>
+        <v>0</v>
       </c>
       <c r="AS15" s="12">
         <v>1</v>
@@ -3235,7 +3235,7 @@
         <v>42409</v>
       </c>
       <c r="AM16" s="2">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AN16" s="2" t="s">
         <v>180</v>
@@ -3244,13 +3244,13 @@
         <v>5</v>
       </c>
       <c r="AP16" s="2">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="AQ16" s="2">
-        <v>3000</v>
+        <v>0</v>
       </c>
       <c r="AR16" s="2">
-        <v>4000</v>
+        <v>0</v>
       </c>
       <c r="AS16" s="12">
         <v>1</v>
@@ -3373,7 +3373,7 @@
         <v>42409</v>
       </c>
       <c r="AM17" s="2">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AN17" s="2" t="s">
         <v>87</v>
@@ -3382,13 +3382,13 @@
         <v>5</v>
       </c>
       <c r="AP17" s="2">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="AQ17" s="2">
-        <v>3000</v>
+        <v>0</v>
       </c>
       <c r="AR17" s="2">
-        <v>4000</v>
+        <v>0</v>
       </c>
       <c r="AS17" s="12">
         <v>1</v>
@@ -3511,7 +3511,7 @@
         <v>42409</v>
       </c>
       <c r="AM18" s="2">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AN18" s="2" t="s">
         <v>87</v>
@@ -3520,13 +3520,13 @@
         <v>5</v>
       </c>
       <c r="AP18" s="2">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="AQ18" s="2">
-        <v>3000</v>
+        <v>0</v>
       </c>
       <c r="AR18" s="2">
-        <v>4000</v>
+        <v>0</v>
       </c>
       <c r="AS18" s="12">
         <v>1</v>
@@ -3649,7 +3649,7 @@
         <v>42409</v>
       </c>
       <c r="AM19" s="2">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AN19" s="2" t="s">
         <v>87</v>
@@ -3658,13 +3658,13 @@
         <v>5</v>
       </c>
       <c r="AP19" s="2">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="AQ19" s="2">
-        <v>3000</v>
+        <v>0</v>
       </c>
       <c r="AR19" s="2">
-        <v>4000</v>
+        <v>0</v>
       </c>
       <c r="AS19" s="12">
         <v>1</v>
@@ -3787,7 +3787,7 @@
         <v>42409</v>
       </c>
       <c r="AM20" s="2">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AN20" s="2" t="s">
         <v>21</v>
@@ -3796,13 +3796,13 @@
         <v>5</v>
       </c>
       <c r="AP20" s="2">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="AQ20" s="2">
-        <v>3000</v>
+        <v>0</v>
       </c>
       <c r="AR20" s="2">
-        <v>4000</v>
+        <v>0</v>
       </c>
       <c r="AS20" s="12">
         <v>1</v>
@@ -3925,7 +3925,7 @@
         <v>42409</v>
       </c>
       <c r="AM21" s="2">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AN21" s="10" t="s">
         <v>181</v>
@@ -3934,13 +3934,13 @@
         <v>132</v>
       </c>
       <c r="AP21" s="2">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="AQ21" s="2">
-        <v>3000</v>
+        <v>0</v>
       </c>
       <c r="AR21" s="2">
-        <v>4000</v>
+        <v>0</v>
       </c>
       <c r="AS21" s="12">
         <v>1</v>
@@ -4062,7 +4062,7 @@
         <v>42409</v>
       </c>
       <c r="AM22" s="2">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AN22" s="2" t="s">
         <v>21</v>
@@ -4071,13 +4071,13 @@
         <v>5</v>
       </c>
       <c r="AP22" s="2">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="AQ22" s="2">
-        <v>3000</v>
+        <v>0</v>
       </c>
       <c r="AR22" s="2">
-        <v>4000</v>
+        <v>0</v>
       </c>
       <c r="AS22" s="12">
         <v>1</v>
@@ -4199,7 +4199,7 @@
         <v>42409</v>
       </c>
       <c r="AM23" s="2">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AN23" s="2" t="s">
         <v>38</v>
@@ -4208,13 +4208,13 @@
         <v>5</v>
       </c>
       <c r="AP23" s="2">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="AQ23" s="2">
-        <v>3000</v>
+        <v>0</v>
       </c>
       <c r="AR23" s="2">
-        <v>4000</v>
+        <v>0</v>
       </c>
       <c r="AS23" s="12">
         <v>1</v>
@@ -4336,7 +4336,7 @@
         <v>42409</v>
       </c>
       <c r="AM24" s="2">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AN24" s="2" t="s">
         <v>38</v>
@@ -4345,13 +4345,13 @@
         <v>5</v>
       </c>
       <c r="AP24" s="2">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="AQ24" s="2">
-        <v>3000</v>
+        <v>0</v>
       </c>
       <c r="AR24" s="2">
-        <v>4000</v>
+        <v>0</v>
       </c>
       <c r="AS24" s="12">
         <v>1</v>

</xml_diff>

<commit_message>
Data master sudah Progress
</commit_message>
<xml_diff>
--- a/public/Excel/MASTER_DATA.xlsx
+++ b/public/Excel/MASTER_DATA.xlsx
@@ -581,7 +581,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yyyy;@"/>
     <numFmt numFmtId="165" formatCode="[$-409]mmm\-yy;@"/>
@@ -1039,8 +1039,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AT51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AD2" workbookViewId="0">
-      <selection activeCell="AM3" sqref="AM3:AM24"/>
+    <sheetView tabSelected="1" topLeftCell="U2" workbookViewId="0">
+      <selection activeCell="Z2" sqref="Z2:Z24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>